<commit_message>
Made Changes for API
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/TestCase.xlsx
+++ b/src/test/resources/ExcelData/TestCase.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC46A339-64D5-4482-8F07-21B2BDDD0986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25273E38-950A-4112-8E8E-1C715EE98EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="1740" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KeywordFramework" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>Keyword</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>CSS</t>
+  </si>
+  <si>
+    <t>Jira</t>
+  </si>
+  <si>
+    <t>Qa-0124</t>
+  </si>
+  <si>
+    <t>Qa-0125</t>
   </si>
 </sst>
 </file>
@@ -438,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,7 +462,7 @@
     <col min="5" max="5" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -469,8 +478,11 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -478,8 +490,11 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -489,8 +504,9 @@
       <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -504,8 +520,9 @@
       <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>7</v>
@@ -519,8 +536,9 @@
       <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -528,8 +546,11 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -539,8 +560,9 @@
       <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>3</v>
@@ -554,8 +576,9 @@
       <c r="E8" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
@@ -569,6 +592,7 @@
       <c r="E9" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="F9" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>